<commit_message>
Change layout of project
</commit_message>
<xml_diff>
--- a/crowd/data/Comments of AtlanticStorm.xlsx
+++ b/crowd/data/Comments of AtlanticStorm.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="316">
   <si>
     <t>id</t>
   </si>
@@ -1684,6 +1684,9 @@
   </si>
   <si>
     <t>Missouri</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -3189,13 +3192,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D39" sqref="D28:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="5" max="5" width="51.6640625" customWidth="1"/>
@@ -4353,7 +4356,7 @@
         <v>121</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>9</v>
+        <v>315</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>139</v>

</xml_diff>